<commit_message>
SAAS-2481 :sparkles: Memoriza aba de ocorrencia e atualiza planilha modelo
</commit_message>
<xml_diff>
--- a/public/Planilha-Modelo-Justto.xlsx
+++ b/public/Planilha-Modelo-Justto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justto CS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E483268D-F946-46B7-9F77-AA6265A0B864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7E1C56-42CF-B548-81B1-1A7A1E1917FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-2085" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27360" yWindow="-4100" windowWidth="33360" windowHeight="17360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Número do processo </t>
   </si>
@@ -56,56 +56,10 @@
     <t xml:space="preserve">Réu </t>
   </si>
   <si>
-    <t>Alçada Máxima</t>
-  </si>
-  <si>
     <t>Data limite - Fim da Negociação</t>
   </si>
   <si>
     <t>Esta planilha é somente um exemplo. Você pode importar planilhas dos formatos .xls .xlsx e .csv com qualquer ordem de colunas, desde que observe as informações abaixo.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Somente os dados da </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monserrat"/>
-      </rPr>
-      <t>primeira aba da planilha</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Monserrat"/>
-      </rPr>
-      <t xml:space="preserve"> serão importados na Plataforma da JUSTTO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Os </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>campos coloridos da planilha principal são obrigatórios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> para a importação. São informações mínimas necessárias para os envios das mensagens. </t>
-    </r>
   </si>
   <si>
     <t>Insira somente uma informação por célula. Nomes e sobrenomes devem estar juntos em uma célula. Prefixos e telefones também devem estar juntos em uma célula.</t>
@@ -122,12 +76,91 @@
   <si>
     <t>Se o caso for extrajudicial, o CPF da parte contrária é o mínimo para importar, pois o sistema irá enriquecer com os dados de contato da pessoa.</t>
   </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>Valor do Pedido</t>
+  </si>
+  <si>
+    <t>Valor Provisionado</t>
+  </si>
+  <si>
+    <t>Vara</t>
+  </si>
+  <si>
+    <t>Comarca</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Subclassificação</t>
+  </si>
+  <si>
+    <t>Valor Dano Moral</t>
+  </si>
+  <si>
+    <t>Valor Dano Material</t>
+  </si>
+  <si>
+    <t>Valor Alçada Máxima</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Somente os dados da </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat Regular"/>
+      </rPr>
+      <t>primeira aba da planilha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat Regular"/>
+      </rPr>
+      <t xml:space="preserve"> serão importados na Plataforma da JUSTTO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Os </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Montserrat Regular"/>
+      </rPr>
+      <t>campos coloridos da planilha principal são obrigatórios</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat Regular"/>
+      </rPr>
+      <t xml:space="preserve"> para a importação. São informações mínimas necessárias para os envios das mensagens. </t>
+    </r>
+  </si>
+  <si>
+    <t>Valor da alçada máxima é o valor máximo que a empresa está disposta a pagar em um acordo, Valor do Pedido é o valor pedido pelo Autor da Ação e Valor Provisionado é o valor que a empresa provisionou para aquela determinada ação judicial.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -145,18 +178,27 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Monserrat"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Montserrat Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Montserrat Regular"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Monserrat"/>
+      <name val="Montserrat Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Montserrat Regular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -179,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -254,11 +296,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -273,23 +343,45 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,344 +738,369 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="13" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="13" customWidth="1"/>
-    <col min="3" max="5" width="14.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="13" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="13"/>
-    <col min="8" max="8" width="23.7109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="18" style="13" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="13"/>
-    <col min="12" max="12" width="18" style="13" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="14.42578125" style="13"/>
+    <col min="1" max="1" width="25.83203125" style="6" customWidth="1"/>
+    <col min="2" max="4" width="14.5" style="6"/>
+    <col min="5" max="5" width="31.1640625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="14.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="6"/>
+    <col min="11" max="11" width="23.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="18" style="6" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="6" customWidth="1"/>
+    <col min="14" max="14" width="14.5" style="6"/>
+    <col min="15" max="15" width="18" style="6" customWidth="1"/>
+    <col min="16" max="20" width="14.5" style="6"/>
+    <col min="21" max="21" width="15.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" style="6"/>
+    <col min="23" max="23" width="29.5" style="6" customWidth="1"/>
+    <col min="24" max="16384" width="14.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="27.75" customHeight="1">
+    <row r="1" spans="1:27" ht="27.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-    </row>
-    <row r="22" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-    </row>
-    <row r="24" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-    </row>
-    <row r="25" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-    </row>
-    <row r="26" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-    </row>
-    <row r="27" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-    </row>
-    <row r="31" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="32" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-    </row>
-    <row r="33" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-    </row>
-    <row r="34" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-    </row>
-    <row r="35" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-    </row>
-    <row r="37" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-    </row>
-    <row r="39" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-    </row>
-    <row r="40" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-    </row>
-    <row r="41" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-    </row>
-    <row r="42" spans="12:13" ht="15.75" customHeight="1">
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-    </row>
-    <row r="43" spans="12:13" ht="15.75" customHeight="1">
-      <c r="M43" s="14"/>
-    </row>
-    <row r="44" spans="12:13" ht="15.75" customHeight="1">
-      <c r="M44" s="14"/>
-    </row>
-    <row r="45" spans="12:13" ht="15.75" customHeight="1">
-      <c r="M45" s="14"/>
-    </row>
-    <row r="46" spans="12:13" ht="15.75" customHeight="1">
-      <c r="M46" s="14"/>
-    </row>
-    <row r="47" spans="12:13" ht="15.75" customHeight="1">
-      <c r="M47" s="14"/>
-    </row>
-    <row r="48" spans="12:13" ht="15.75" customHeight="1">
-      <c r="M48" s="14"/>
-    </row>
-    <row r="49" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M49" s="14"/>
-    </row>
-    <row r="50" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M50" s="14"/>
-    </row>
-    <row r="51" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M51" s="14"/>
-    </row>
-    <row r="52" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M52" s="14"/>
-    </row>
-    <row r="53" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M53" s="14"/>
-    </row>
-    <row r="54" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M54" s="14"/>
-    </row>
-    <row r="55" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M55" s="14"/>
-    </row>
-    <row r="56" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M56" s="14"/>
-    </row>
-    <row r="57" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M57" s="14"/>
-    </row>
-    <row r="58" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M58" s="14"/>
-    </row>
-    <row r="59" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M59" s="14"/>
-    </row>
-    <row r="60" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M60" s="14"/>
-    </row>
-    <row r="61" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M61" s="14"/>
-    </row>
-    <row r="62" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M62" s="14"/>
-    </row>
-    <row r="63" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M63" s="14"/>
-    </row>
-    <row r="64" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M64" s="14"/>
-    </row>
-    <row r="65" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M65" s="14"/>
-    </row>
-    <row r="66" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M66" s="14"/>
-    </row>
-    <row r="67" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M67" s="14"/>
-    </row>
-    <row r="68" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M68" s="14"/>
-    </row>
-    <row r="69" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M69" s="14"/>
-    </row>
-    <row r="70" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M70" s="14"/>
-    </row>
-    <row r="71" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M71" s="14"/>
-    </row>
-    <row r="72" spans="13:13" ht="15.75" customHeight="1">
-      <c r="M72" s="14"/>
-    </row>
-    <row r="73" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="74" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="75" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="76" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="77" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="78" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="79" spans="13:13" ht="15.75" customHeight="1"/>
-    <row r="80" spans="13:13" ht="15.75" customHeight="1"/>
+      <c r="AA1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O2" s="7"/>
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O4" s="7"/>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O5" s="7"/>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O6" s="7"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O7" s="7"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O8" s="7"/>
+      <c r="W8" s="7"/>
+    </row>
+    <row r="9" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O9" s="7"/>
+      <c r="W9" s="7"/>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O10" s="7"/>
+      <c r="W10" s="7"/>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O11" s="7"/>
+      <c r="W11" s="7"/>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O12" s="7"/>
+      <c r="W12" s="7"/>
+    </row>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O13" s="7"/>
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O14" s="7"/>
+      <c r="W14" s="7"/>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O15" s="7"/>
+      <c r="W15" s="7"/>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
+      <c r="O16" s="7"/>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O17" s="7"/>
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O18" s="7"/>
+      <c r="W18" s="7"/>
+    </row>
+    <row r="19" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O19" s="7"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O20" s="7"/>
+      <c r="W20" s="7"/>
+    </row>
+    <row r="21" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O21" s="7"/>
+      <c r="W21" s="7"/>
+    </row>
+    <row r="22" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O22" s="7"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O23" s="7"/>
+      <c r="W23" s="7"/>
+    </row>
+    <row r="24" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O24" s="7"/>
+      <c r="W24" s="7"/>
+    </row>
+    <row r="25" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O25" s="7"/>
+      <c r="W25" s="7"/>
+    </row>
+    <row r="26" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O26" s="7"/>
+      <c r="W26" s="7"/>
+    </row>
+    <row r="27" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O27" s="7"/>
+      <c r="W27" s="7"/>
+    </row>
+    <row r="28" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O28" s="7"/>
+      <c r="W28" s="7"/>
+    </row>
+    <row r="29" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O29" s="7"/>
+      <c r="W29" s="7"/>
+    </row>
+    <row r="30" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O30" s="7"/>
+      <c r="W30" s="7"/>
+    </row>
+    <row r="31" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O31" s="7"/>
+      <c r="W31" s="7"/>
+    </row>
+    <row r="32" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O32" s="7"/>
+      <c r="W32" s="7"/>
+    </row>
+    <row r="33" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O33" s="7"/>
+      <c r="W33" s="7"/>
+    </row>
+    <row r="34" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O34" s="7"/>
+      <c r="W34" s="7"/>
+    </row>
+    <row r="35" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O35" s="7"/>
+      <c r="W35" s="7"/>
+    </row>
+    <row r="36" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O36" s="7"/>
+      <c r="W36" s="7"/>
+    </row>
+    <row r="37" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O37" s="7"/>
+      <c r="W37" s="7"/>
+    </row>
+    <row r="38" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O38" s="7"/>
+      <c r="W38" s="7"/>
+    </row>
+    <row r="39" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O39" s="7"/>
+      <c r="W39" s="7"/>
+    </row>
+    <row r="40" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O40" s="7"/>
+      <c r="W40" s="7"/>
+    </row>
+    <row r="41" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O41" s="7"/>
+      <c r="W41" s="7"/>
+    </row>
+    <row r="42" spans="15:23" ht="15.75" customHeight="1">
+      <c r="O42" s="7"/>
+      <c r="W42" s="7"/>
+    </row>
+    <row r="43" spans="15:23" ht="15.75" customHeight="1">
+      <c r="W43" s="7"/>
+    </row>
+    <row r="44" spans="15:23" ht="15.75" customHeight="1">
+      <c r="W44" s="7"/>
+    </row>
+    <row r="45" spans="15:23" ht="15.75" customHeight="1">
+      <c r="W45" s="7"/>
+    </row>
+    <row r="46" spans="15:23" ht="15.75" customHeight="1">
+      <c r="W46" s="7"/>
+    </row>
+    <row r="47" spans="15:23" ht="15.75" customHeight="1">
+      <c r="W47" s="7"/>
+    </row>
+    <row r="48" spans="15:23" ht="15.75" customHeight="1">
+      <c r="W48" s="7"/>
+    </row>
+    <row r="49" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W49" s="7"/>
+    </row>
+    <row r="50" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W50" s="7"/>
+    </row>
+    <row r="51" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W51" s="7"/>
+    </row>
+    <row r="52" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W52" s="7"/>
+    </row>
+    <row r="53" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W53" s="7"/>
+    </row>
+    <row r="54" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W54" s="7"/>
+    </row>
+    <row r="55" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W55" s="7"/>
+    </row>
+    <row r="56" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W56" s="7"/>
+    </row>
+    <row r="57" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W57" s="7"/>
+    </row>
+    <row r="58" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W58" s="7"/>
+    </row>
+    <row r="59" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W59" s="7"/>
+    </row>
+    <row r="60" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W60" s="7"/>
+    </row>
+    <row r="61" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W61" s="7"/>
+    </row>
+    <row r="62" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W62" s="7"/>
+    </row>
+    <row r="63" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W63" s="7"/>
+    </row>
+    <row r="64" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W64" s="7"/>
+    </row>
+    <row r="65" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W65" s="7"/>
+    </row>
+    <row r="66" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W66" s="7"/>
+    </row>
+    <row r="67" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W67" s="7"/>
+    </row>
+    <row r="68" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W68" s="7"/>
+    </row>
+    <row r="69" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W69" s="7"/>
+    </row>
+    <row r="70" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W70" s="7"/>
+    </row>
+    <row r="71" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W71" s="7"/>
+    </row>
+    <row r="72" spans="23:23" ht="15.75" customHeight="1">
+      <c r="W72" s="7"/>
+    </row>
+    <row r="73" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="74" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="75" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="76" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="77" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="78" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="79" spans="23:23" ht="15.75" customHeight="1"/>
+    <row r="80" spans="23:23" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -1914,11 +2031,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:R34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
@@ -2145,461 +2264,461 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="12.75" customHeight="1">
+    <row r="9" spans="1:26" ht="16">
       <c r="A9" s="2"/>
-      <c r="B9" s="8" t="s">
-        <v>13</v>
+      <c r="B9" s="17" t="s">
+        <v>12</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="12.75" customHeight="1">
+    <row r="10" spans="1:26" ht="16">
       <c r="A10" s="2"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="12.75" customHeight="1">
+    <row r="11" spans="1:26" ht="16" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="8" t="s">
-        <v>14</v>
+      <c r="B11" s="17" t="s">
+        <v>29</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="19"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="12.75" customHeight="1">
+    <row r="12" spans="1:26" ht="16">
       <c r="A12" s="2"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" ht="12.75" customHeight="1">
+    <row r="13" spans="1:26" ht="16" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="11" t="s">
-        <v>15</v>
+      <c r="B13" s="22"/>
+      <c r="C13" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="19"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26" ht="12.75" customHeight="1">
+    <row r="14" spans="1:26" ht="16">
       <c r="A14" s="2"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1">
+    <row r="15" spans="1:26" ht="16" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="8" t="s">
-        <v>16</v>
+      <c r="B15" s="17" t="s">
+        <v>13</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="19"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1">
+    <row r="16" spans="1:26" ht="16">
       <c r="A16" s="2"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="12.75" customHeight="1">
+    <row r="17" spans="1:26" ht="16" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="8" t="s">
-        <v>17</v>
+      <c r="B17" s="17" t="s">
+        <v>14</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="19"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" ht="12.75" customHeight="1">
+    <row r="18" spans="1:26" ht="16">
       <c r="A18" s="2"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" ht="12.75" customHeight="1">
+    <row r="19" spans="1:26" ht="16" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="12" t="s">
-        <v>18</v>
+      <c r="B19" s="17" t="s">
+        <v>15</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="19"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26" ht="12.75" customHeight="1">
+    <row r="20" spans="1:26" ht="16">
       <c r="A20" s="2"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="29.25" customHeight="1">
+    <row r="21" spans="1:26" ht="16" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" s="12" t="s">
-        <v>19</v>
+      <c r="B21" s="17" t="s">
+        <v>16</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="19"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" ht="12.75" customHeight="1">
+    <row r="23" spans="1:26" ht="16" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="8" t="s">
-        <v>20</v>
+      <c r="B23" s="17" t="s">
+        <v>17</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="19"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="10"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="16"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
@@ -2609,29 +2728,31 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="12.75" customHeight="1">
+    <row r="25" spans="1:26" ht="37" customHeight="1">
       <c r="A25" s="2"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
+      <c r="B25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
@@ -2639,7 +2760,7 @@
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -2667,7 +2788,7 @@
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1">
       <c r="A27" s="2"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -2695,7 +2816,7 @@
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -2723,7 +2844,7 @@
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1">
       <c r="A29" s="2"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -2751,7 +2872,7 @@
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -2779,7 +2900,7 @@
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1">
       <c r="A31" s="2"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -2807,7 +2928,7 @@
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -2835,7 +2956,7 @@
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="11"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -2863,7 +2984,7 @@
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1">
       <c r="A34" s="2"/>
-      <c r="B34" s="11"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -2891,7 +3012,7 @@
     </row>
     <row r="35" spans="1:26" ht="12.75" customHeight="1">
       <c r="A35" s="2"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -2919,7 +3040,7 @@
     </row>
     <row r="36" spans="1:26" ht="12.75" customHeight="1">
       <c r="A36" s="2"/>
-      <c r="B36" s="11"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -2947,7 +3068,7 @@
     </row>
     <row r="37" spans="1:26" ht="12.75" customHeight="1">
       <c r="A37" s="2"/>
-      <c r="B37" s="11"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -2975,7 +3096,7 @@
     </row>
     <row r="38" spans="1:26" ht="12.75" customHeight="1">
       <c r="A38" s="2"/>
-      <c r="B38" s="11"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -3003,7 +3124,7 @@
     </row>
     <row r="39" spans="1:26" ht="12.75" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="11"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -3031,7 +3152,7 @@
     </row>
     <row r="40" spans="1:26" ht="12.75" customHeight="1">
       <c r="A40" s="2"/>
-      <c r="B40" s="11"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -3059,7 +3180,7 @@
     </row>
     <row r="41" spans="1:26" ht="12.75" customHeight="1">
       <c r="A41" s="2"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -3087,7 +3208,7 @@
     </row>
     <row r="42" spans="1:26" ht="12.75" customHeight="1">
       <c r="A42" s="2"/>
-      <c r="B42" s="11"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -3115,7 +3236,7 @@
     </row>
     <row r="43" spans="1:26" ht="12.75" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="11"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -3143,7 +3264,7 @@
     </row>
     <row r="44" spans="1:26" ht="12.75" customHeight="1">
       <c r="A44" s="2"/>
-      <c r="B44" s="11"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -3171,7 +3292,7 @@
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1">
       <c r="A45" s="2"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -3199,7 +3320,7 @@
     </row>
     <row r="46" spans="1:26" ht="12.75" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="11"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -3227,7 +3348,7 @@
     </row>
     <row r="47" spans="1:26" ht="12.75" customHeight="1">
       <c r="A47" s="2"/>
-      <c r="B47" s="11"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -3255,7 +3376,7 @@
     </row>
     <row r="48" spans="1:26" ht="12.75" customHeight="1">
       <c r="A48" s="2"/>
-      <c r="B48" s="11"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -3283,7 +3404,7 @@
     </row>
     <row r="49" spans="1:26" ht="12.75" customHeight="1">
       <c r="A49" s="2"/>
-      <c r="B49" s="11"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
@@ -29995,12 +30116,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B31:R31"/>
-    <mergeCell ref="B30:R30"/>
-    <mergeCell ref="B37:R37"/>
-    <mergeCell ref="B38:R38"/>
-    <mergeCell ref="B39:R39"/>
-    <mergeCell ref="B36:R36"/>
+    <mergeCell ref="B9:W9"/>
+    <mergeCell ref="B11:V11"/>
+    <mergeCell ref="C13:V13"/>
+    <mergeCell ref="B15:V15"/>
+    <mergeCell ref="B17:V17"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B16:R16"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="B27:R27"/>
+    <mergeCell ref="B19:V19"/>
+    <mergeCell ref="B21:V21"/>
+    <mergeCell ref="B23:V23"/>
+    <mergeCell ref="B25:V25"/>
     <mergeCell ref="B49:R49"/>
     <mergeCell ref="B43:R43"/>
     <mergeCell ref="B44:R44"/>
@@ -30015,27 +30148,200 @@
     <mergeCell ref="B46:R46"/>
     <mergeCell ref="B47:R47"/>
     <mergeCell ref="B48:R48"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B19:R19"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="B27:R27"/>
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B15:R15"/>
-    <mergeCell ref="B16:R16"/>
-    <mergeCell ref="C13:P13"/>
-    <mergeCell ref="B17:R17"/>
+    <mergeCell ref="B31:R31"/>
+    <mergeCell ref="B30:R30"/>
+    <mergeCell ref="B37:R37"/>
+    <mergeCell ref="B38:R38"/>
+    <mergeCell ref="B39:R39"/>
+    <mergeCell ref="B36:R36"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100327A0A16451B014ABDA578C848F587FB" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0108617b17f8ffbf86121e7927ab083b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e56d2328-2fe0-4298-ae7c-820747856993" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4d4e3f8e815236e76de05d1d5a42c4f" ns2:_="">
+    <xsd:import namespace="e56d2328-2fe0-4298-ae7c-820747856993"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e56d2328-2fe0-4298-ae7c-820747856993" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF4B4999-D20A-4313-9583-CC354D497006}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817DEC52-9993-4A84-9FF2-DACD5DA36F2F}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFE81249-2F31-4B97-BD45-109D86009232}"/>
 </file>
</xml_diff>